<commit_message>
Succesfully integrated Applying scenarios on a single sheet to make analytics easier
</commit_message>
<xml_diff>
--- a/simulate_and_return_the_data_in_xlsx_format/Etherium Long LP Strategy Simulation.xlsx
+++ b/simulate_and_return_the_data_in_xlsx_format/Etherium Long LP Strategy Simulation.xlsx
@@ -6,6 +6,7 @@
     <sheet name="README" sheetId="1" r:id="rId1"/>
     <sheet name="Scenario 1 - Gradual Increase" sheetId="2" r:id="rId2"/>
     <sheet name="Scenario 2 - Gradual Decrease" sheetId="3" r:id="rId3"/>
+    <sheet name="Combined Scenarios" sheetId="4" r:id="rId4"/>
   </sheets>
 </workbook>
 </file>
@@ -399,7 +400,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C19"/>
+  <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -417,1689 +418,3267 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>Month</v>
+        <v>Scenario</v>
       </c>
       <c r="B2" t="str">
-        <v>Represents the month number in the simulation (1-12).</v>
+        <v>ETH price scenario name</v>
       </c>
       <c r="C2" t="str">
-        <v>Incremental: 1 through 12</v>
+        <v>One of the defined scenarios</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>ETH Price at Deposit ($/ETH)</v>
+        <v>Month</v>
       </c>
       <c r="B3" t="str">
-        <v>The ETH price at the end of the month used for deposit.</v>
+        <v>Represents the month number in the simulation (1-12).</v>
       </c>
       <c r="C3" t="str">
-        <v>From ETH price scenario object</v>
+        <v>Incremental: 1 through 12</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>Deposit Amount ($)</v>
+        <v>ETH Price at Deposit ($/ETH)</v>
       </c>
       <c r="B4" t="str">
-        <v>The amount of money invested monthly in USD.</v>
+        <v>The ETH price at the end of the month used for deposit.</v>
       </c>
       <c r="C4" t="str">
-        <v>Constant: $150</v>
+        <v>From ETH price scenario object</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v>Total ETH Held Without Interest (ETH)</v>
+        <v>Deposit Amount ($)</v>
       </c>
       <c r="B5" t="str">
-        <v>Total accumulated ETH from deposits, without compounding interest.</v>
+        <v>The amount of money invested monthly in USD.</v>
       </c>
       <c r="C5" t="str">
-        <v>Σ (Deposit Amount / ETH Price)</v>
+        <v>Constant: $150</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="str">
-        <v>Total ETH Held With Interest (ETH)</v>
+        <v>Total ETH Held Without Interest (ETH)</v>
       </c>
       <c r="B6" t="str">
-        <v>Total ETH including monthly compounding interest.</v>
+        <v>Total accumulated ETH from deposits, without compounding interest.</v>
       </c>
       <c r="C6" t="str">
-        <v>(Previous ETH + new ETH) * (1 + monthlyInterestRate)</v>
+        <v>Σ (Deposit Amount / ETH Price)</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="str">
-        <v>Total ETH Value (USD)</v>
+        <v>Total ETH Held With Interest (ETH)</v>
       </c>
       <c r="B7" t="str">
-        <v>Value of total ETH held (with interest) at current ETH price.</v>
+        <v>Total ETH including monthly compounding interest.</v>
       </c>
       <c r="C7" t="str">
-        <v>Total ETH With Interest * ETH Price</v>
+        <v>(Previous ETH + new ETH) * (1 + monthlyInterestRate)</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="str">
-        <v>Borrowed Amount (This Month, $)</v>
+        <v>Total ETH Value (USD)</v>
       </c>
       <c r="B8" t="str">
-        <v>The new borrowed amount to maintain a 45% LTV in this month.</v>
+        <v>Value of total ETH held (with interest) at current ETH price.</v>
       </c>
       <c r="C8" t="str">
-        <v>(Total Capital * 0.45) - Total Borrowed</v>
+        <v>Total ETH With Interest * ETH Price</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="str">
-        <v>Total Borrowed with Interest ($)</v>
+        <v>Borrowed Amount (This Month, $)</v>
       </c>
       <c r="B9" t="str">
-        <v>Total borrowed amount accumulated with interest.</v>
+        <v>The new borrowed amount to maintain a 45% LTV in this month.</v>
       </c>
       <c r="C9" t="str">
-        <v>(Previous Total Borrowed + This Month Borrowed) * (1 + monthlyInterestRate)</v>
+        <v>(Total Capital * 0.45) - Total Borrowed</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="str">
-        <v>Borrow Rate (%)</v>
+        <v>Total Borrowed with Interest ($)</v>
       </c>
       <c r="B10" t="str">
-        <v>Borrowed amount for this month as a percentage of capital.</v>
+        <v>Total borrowed amount accumulated with interest.</v>
       </c>
       <c r="C10" t="str">
-        <v>(This Month Borrowed / Total Capital) * 100</v>
+        <v>(Previous Total Borrowed + This Month Borrowed) * (1 + monthlyInterestRate)</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="str">
-        <v>LTV (%)</v>
+        <v>Borrow Rate (%)</v>
       </c>
       <c r="B11" t="str">
-        <v>Loan-to-Value ratio based on current capital.</v>
+        <v>Borrowed amount for this month as a percentage of capital.</v>
       </c>
       <c r="C11" t="str">
-        <v>(Total Borrowed / Total Capital) * 100</v>
+        <v>(This Month Borrowed / Total Capital) * 100</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="str">
-        <v>LP Growth ($)</v>
+        <v>LTV (%)</v>
       </c>
       <c r="B12" t="str">
-        <v>Cumulative growth of funds added to LP using borrowed capital.</v>
+        <v>Loan-to-Value ratio based on current capital.</v>
       </c>
       <c r="C12" t="str">
-        <v>Σ (This Month Borrowed)</v>
+        <v>(Total Borrowed / Total Capital) * 100</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="str">
-        <v>Impermanent Loss (%)</v>
+        <v>LP Growth ($)</v>
       </c>
       <c r="B13" t="str">
-        <v>Impermanent loss percentage due to ETH price divergence from original price ($2200).</v>
+        <v>Cumulative growth of funds added to LP using borrowed capital.</v>
       </c>
       <c r="C13" t="str">
-        <v>1 - (2 * √(p1/p0)) / (1 + p1/p0)</v>
+        <v>Σ (This Month Borrowed)</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="str">
-        <v>LP Value After IL ($)</v>
+        <v>Impermanent Loss (%)</v>
       </c>
       <c r="B14" t="str">
-        <v>Liquidity Pool value after applying impermanent loss.</v>
+        <v>Impermanent loss percentage due to ETH price divergence from original price ($2200).</v>
       </c>
       <c r="C14" t="str">
-        <v>LP Growth * (1 - IL)</v>
+        <v>1 - (2 * √(p1/p0)) / (1 + p1/p0)</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="str">
-        <v>Gas Fee (Base Chain) ($)</v>
+        <v>LP Value After IL ($)</v>
       </c>
       <c r="B15" t="str">
-        <v>Fixed gas fees paid monthly (lend, borrow, LP) on the Base chain.</v>
+        <v>Liquidity Pool value after applying impermanent loss.</v>
       </c>
       <c r="C15" t="str">
-        <v>0.02 + 0.03 + 0.05</v>
+        <v>LP Growth * (1 - IL)</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="str">
-        <v>Net Capital ($)</v>
+        <v>Gas Fee (Base Chain) ($)</v>
       </c>
       <c r="B16" t="str">
-        <v>Final capital after adding ETH value, LP, deducting gas and debt.</v>
+        <v>Fixed gas fees paid monthly (lend, borrow, LP) on the Base chain.</v>
       </c>
       <c r="C16" t="str">
-        <v>ETH Value + LP Value - Total Borrowed - Gas Fee</v>
+        <v>0.02 + 0.03 + 0.05</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="str">
-        <v>ETH Liquidation Price ($)</v>
+        <v>Net Capital ($)</v>
       </c>
       <c r="B17" t="str">
-        <v>Price at which ETH would trigger liquidation based on current LTV.</v>
+        <v>Final capital after adding ETH value, LP, deducting gas and debt.</v>
       </c>
       <c r="C17" t="str">
-        <v>(Total Borrowed * 0.825) / Total ETH Held</v>
+        <v>ETH Value + LP Value - Total Borrowed - Gas Fee</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="str">
-        <v>Liquidated?</v>
+        <v>ETH Liquidation Price ($)</v>
       </c>
       <c r="B18" t="str">
-        <v>Whether your position would be liquidated this month ('Yes' or 'No').</v>
+        <v>Price at which ETH would trigger liquidation based on current LTV.</v>
       </c>
       <c r="C18" t="str">
-        <v>Yes if LTV &gt; 82.5%, else No</v>
+        <v>(Total Borrowed * 0.825) / Total ETH Held</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="str">
+        <v>Liquidated?</v>
+      </c>
+      <c r="B19" t="str">
+        <v>Whether your position would be liquidated this month ('Yes' or 'No').</v>
+      </c>
+      <c r="C19" t="str">
+        <v>Yes if LTV &gt; 82.5%, else No</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="str">
         <v>Profit ($)</v>
       </c>
-      <c r="B19" t="str">
+      <c r="B20" t="str">
         <v>Net capital + LP - Total Deposits, representing final profit/loss.</v>
       </c>
-      <c r="C19" t="str">
+      <c r="C20" t="str">
         <v>Net Capital - Total Deposits + LP Value</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:C19"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:C20"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:R13"/>
+  <dimension ref="A1:S13"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
+        <v>Scenario</v>
+      </c>
+      <c r="B1" t="str">
         <v>Month</v>
       </c>
-      <c r="B1" t="str">
+      <c r="C1" t="str">
         <v>ETH Price at Deposit ($/ETH)</v>
       </c>
-      <c r="C1" t="str">
+      <c r="D1" t="str">
         <v>Deposit Amount ($)</v>
       </c>
-      <c r="D1" t="str">
+      <c r="E1" t="str">
         <v>Total ETH Held Without Interest (ETH)</v>
       </c>
-      <c r="E1" t="str">
+      <c r="F1" t="str">
         <v>Total ETH Held With Interest (ETH)</v>
       </c>
-      <c r="F1" t="str">
+      <c r="G1" t="str">
         <v>Total ETH Value (USD)</v>
       </c>
-      <c r="G1" t="str">
+      <c r="H1" t="str">
         <v>Borrowed Amount (This Month, $)</v>
       </c>
-      <c r="H1" t="str">
+      <c r="I1" t="str">
         <v>Total Borrowed with Interest ($)</v>
       </c>
-      <c r="I1" t="str">
+      <c r="J1" t="str">
         <v>Borrow Rate (%)</v>
       </c>
-      <c r="J1" t="str">
+      <c r="K1" t="str">
         <v>LTV (%)</v>
       </c>
-      <c r="K1" t="str">
+      <c r="L1" t="str">
         <v>LP Growth ($)</v>
       </c>
-      <c r="L1" t="str">
+      <c r="M1" t="str">
         <v>Impermanent Loss (%)</v>
       </c>
-      <c r="M1" t="str">
+      <c r="N1" t="str">
         <v>LP Value After IL ($)</v>
       </c>
-      <c r="N1" t="str">
+      <c r="O1" t="str">
         <v>Gas Fee (Base Chain) ($)</v>
       </c>
-      <c r="O1" t="str">
+      <c r="P1" t="str">
         <v>Net Capital ($)</v>
       </c>
-      <c r="P1" t="str">
+      <c r="Q1" t="str">
         <v>ETH Liquidation Price ($)</v>
       </c>
-      <c r="Q1" t="str">
+      <c r="R1" t="str">
         <v>Liquidated?</v>
       </c>
-      <c r="R1" t="str">
+      <c r="S1" t="str">
         <v>Profit ($)</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2">
+      <c r="A2" t="str">
+        <v>Scenario 1 - Gradual Increase</v>
+      </c>
+      <c r="B2">
         <v>1</v>
       </c>
-      <c r="B2">
+      <c r="C2">
         <v>2200</v>
       </c>
-      <c r="C2" t="str">
-        <v>150.00</v>
-      </c>
       <c r="D2" t="str">
+        <v>150.00</v>
+      </c>
+      <c r="E2" t="str">
         <v>0.068182</v>
       </c>
-      <c r="E2" t="str">
+      <c r="F2" t="str">
         <v>0.068295</v>
       </c>
-      <c r="F2" t="str">
+      <c r="G2" t="str">
         <v>150.25</v>
       </c>
-      <c r="G2" t="str">
+      <c r="H2" t="str">
         <v>67.61</v>
       </c>
-      <c r="H2" t="str">
+      <c r="I2" t="str">
         <v>67.73</v>
       </c>
-      <c r="I2" t="str">
+      <c r="J2" t="str">
         <v>45.00</v>
       </c>
-      <c r="J2" t="str">
-        <v>45.08</v>
-      </c>
       <c r="K2" t="str">
+        <v>45.08</v>
+      </c>
+      <c r="L2" t="str">
         <v>67.61</v>
       </c>
-      <c r="L2" t="str">
+      <c r="M2" t="str">
         <v>0.00</v>
       </c>
-      <c r="M2" t="str">
+      <c r="N2" t="str">
         <v>67.61</v>
       </c>
-      <c r="N2" t="str">
-        <v>0.10</v>
-      </c>
       <c r="O2" t="str">
+        <v>0.10</v>
+      </c>
+      <c r="P2" t="str">
         <v>150.04</v>
       </c>
-      <c r="P2" t="str">
+      <c r="Q2" t="str">
         <v>818.11</v>
       </c>
-      <c r="Q2" t="str">
-        <v>No</v>
-      </c>
       <c r="R2" t="str">
+        <v>No</v>
+      </c>
+      <c r="S2" t="str">
         <v>67.65</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3">
+      <c r="A3" t="str">
+        <v>Scenario 1 - Gradual Increase</v>
+      </c>
+      <c r="B3">
         <v>2</v>
       </c>
-      <c r="B3">
+      <c r="C3">
         <v>2200</v>
       </c>
-      <c r="C3" t="str">
-        <v>150.00</v>
-      </c>
       <c r="D3" t="str">
+        <v>150.00</v>
+      </c>
+      <c r="E3" t="str">
         <v>0.136364</v>
       </c>
-      <c r="E3" t="str">
+      <c r="F3" t="str">
         <v>0.136705</v>
       </c>
-      <c r="F3" t="str">
+      <c r="G3" t="str">
         <v>300.75</v>
       </c>
-      <c r="G3" t="str">
+      <c r="H3" t="str">
         <v>98.04</v>
       </c>
-      <c r="H3" t="str">
+      <c r="I3" t="str">
         <v>166.04</v>
       </c>
-      <c r="I3" t="str">
+      <c r="J3" t="str">
         <v>26.61</v>
       </c>
-      <c r="J3" t="str">
-        <v>45.08</v>
-      </c>
       <c r="K3" t="str">
+        <v>45.08</v>
+      </c>
+      <c r="L3" t="str">
         <v>165.65</v>
       </c>
-      <c r="L3" t="str">
+      <c r="M3" t="str">
         <v>0.00</v>
       </c>
-      <c r="M3" t="str">
+      <c r="N3" t="str">
         <v>165.65</v>
       </c>
-      <c r="N3" t="str">
-        <v>0.10</v>
-      </c>
       <c r="O3" t="str">
+        <v>0.10</v>
+      </c>
+      <c r="P3" t="str">
         <v>300.26</v>
       </c>
-      <c r="P3" t="str">
+      <c r="Q3" t="str">
         <v>1002.03</v>
       </c>
-      <c r="Q3" t="str">
-        <v>No</v>
-      </c>
       <c r="R3" t="str">
+        <v>No</v>
+      </c>
+      <c r="S3" t="str">
         <v>165.91</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4">
+      <c r="A4" t="str">
+        <v>Scenario 1 - Gradual Increase</v>
+      </c>
+      <c r="B4">
         <v>3</v>
       </c>
-      <c r="B4">
+      <c r="C4">
         <v>2200</v>
       </c>
-      <c r="C4" t="str">
-        <v>150.00</v>
-      </c>
       <c r="D4" t="str">
+        <v>150.00</v>
+      </c>
+      <c r="E4" t="str">
         <v>0.204545</v>
       </c>
-      <c r="E4" t="str">
+      <c r="F4" t="str">
         <v>0.205228</v>
       </c>
-      <c r="F4" t="str">
+      <c r="G4" t="str">
         <v>451.50</v>
       </c>
-      <c r="G4" t="str">
+      <c r="H4" t="str">
         <v>111.68</v>
       </c>
-      <c r="H4" t="str">
+      <c r="I4" t="str">
         <v>278.18</v>
       </c>
-      <c r="I4" t="str">
+      <c r="J4" t="str">
         <v>18.10</v>
       </c>
-      <c r="J4" t="str">
-        <v>45.08</v>
-      </c>
       <c r="K4" t="str">
+        <v>45.08</v>
+      </c>
+      <c r="L4" t="str">
         <v>277.33</v>
       </c>
-      <c r="L4" t="str">
+      <c r="M4" t="str">
         <v>0.00</v>
       </c>
-      <c r="M4" t="str">
+      <c r="N4" t="str">
         <v>277.33</v>
       </c>
-      <c r="N4" t="str">
-        <v>0.10</v>
-      </c>
       <c r="O4" t="str">
+        <v>0.10</v>
+      </c>
+      <c r="P4" t="str">
         <v>450.55</v>
       </c>
-      <c r="P4" t="str">
+      <c r="Q4" t="str">
         <v>1118.27</v>
       </c>
-      <c r="Q4" t="str">
-        <v>No</v>
-      </c>
       <c r="R4" t="str">
+        <v>No</v>
+      </c>
+      <c r="S4" t="str">
         <v>277.88</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5">
+      <c r="A5" t="str">
+        <v>Scenario 1 - Gradual Increase</v>
+      </c>
+      <c r="B5">
         <v>4</v>
       </c>
-      <c r="B5">
+      <c r="C5">
         <v>2800</v>
       </c>
-      <c r="C5" t="str">
-        <v>150.00</v>
-      </c>
       <c r="D5" t="str">
+        <v>150.00</v>
+      </c>
+      <c r="E5" t="str">
         <v>0.258117</v>
       </c>
-      <c r="E5" t="str">
+      <c r="F5" t="str">
         <v>0.259231</v>
       </c>
-      <c r="F5" t="str">
+      <c r="G5" t="str">
         <v>725.85</v>
       </c>
-      <c r="G5" t="str">
+      <c r="H5" t="str">
         <v>173.25</v>
       </c>
-      <c r="H5" t="str">
+      <c r="I5" t="str">
         <v>452.18</v>
       </c>
-      <c r="I5" t="str">
+      <c r="J5" t="str">
         <v>17.27</v>
       </c>
-      <c r="J5" t="str">
-        <v>45.08</v>
-      </c>
       <c r="K5" t="str">
+        <v>45.08</v>
+      </c>
+      <c r="L5" t="str">
         <v>450.58</v>
       </c>
-      <c r="L5" t="str">
+      <c r="M5" t="str">
         <v>0.72</v>
       </c>
-      <c r="M5" t="str">
+      <c r="N5" t="str">
         <v>447.32</v>
       </c>
-      <c r="N5" t="str">
-        <v>0.10</v>
-      </c>
       <c r="O5" t="str">
+        <v>0.10</v>
+      </c>
+      <c r="P5" t="str">
         <v>720.89</v>
       </c>
-      <c r="P5" t="str">
+      <c r="Q5" t="str">
         <v>1439.06</v>
       </c>
-      <c r="Q5" t="str">
-        <v>No</v>
-      </c>
       <c r="R5" t="str">
+        <v>No</v>
+      </c>
+      <c r="S5" t="str">
         <v>568.21</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6">
+      <c r="A6" t="str">
+        <v>Scenario 1 - Gradual Increase</v>
+      </c>
+      <c r="B6">
         <v>5</v>
       </c>
-      <c r="B6">
+      <c r="C6">
         <v>2800</v>
       </c>
-      <c r="C6" t="str">
-        <v>150.00</v>
-      </c>
       <c r="D6" t="str">
+        <v>150.00</v>
+      </c>
+      <c r="E6" t="str">
         <v>0.311688</v>
       </c>
-      <c r="E6" t="str">
+      <c r="F6" t="str">
         <v>0.313324</v>
       </c>
-      <c r="F6" t="str">
+      <c r="G6" t="str">
         <v>877.31</v>
       </c>
-      <c r="G6" t="str">
+      <c r="H6" t="str">
         <v>145.37</v>
       </c>
-      <c r="H6" t="str">
+      <c r="I6" t="str">
         <v>598.54</v>
       </c>
-      <c r="I6" t="str">
+      <c r="J6" t="str">
         <v>10.95</v>
       </c>
-      <c r="J6" t="str">
+      <c r="K6" t="str">
         <v>45.07</v>
       </c>
-      <c r="K6" t="str">
+      <c r="L6" t="str">
         <v>595.94</v>
       </c>
-      <c r="L6" t="str">
+      <c r="M6" t="str">
         <v>0.72</v>
       </c>
-      <c r="M6" t="str">
+      <c r="N6" t="str">
         <v>591.64</v>
       </c>
-      <c r="N6" t="str">
-        <v>0.10</v>
-      </c>
       <c r="O6" t="str">
+        <v>0.10</v>
+      </c>
+      <c r="P6" t="str">
         <v>870.30</v>
       </c>
-      <c r="P6" t="str">
+      <c r="Q6" t="str">
         <v>1576.00</v>
       </c>
-      <c r="Q6" t="str">
-        <v>No</v>
-      </c>
       <c r="R6" t="str">
+        <v>No</v>
+      </c>
+      <c r="S6" t="str">
         <v>711.94</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7">
+      <c r="A7" t="str">
+        <v>Scenario 1 - Gradual Increase</v>
+      </c>
+      <c r="B7">
         <v>6</v>
       </c>
-      <c r="B7">
+      <c r="C7">
         <v>2800</v>
       </c>
-      <c r="C7" t="str">
-        <v>150.00</v>
-      </c>
       <c r="D7" t="str">
+        <v>150.00</v>
+      </c>
+      <c r="E7" t="str">
         <v>0.365260</v>
       </c>
-      <c r="E7" t="str">
+      <c r="F7" t="str">
         <v>0.367506</v>
       </c>
-      <c r="F7" t="str">
+      <c r="G7" t="str">
         <v>1029.02</v>
       </c>
-      <c r="G7" t="str">
+      <c r="H7" t="str">
         <v>132.69</v>
       </c>
-      <c r="H7" t="str">
+      <c r="I7" t="str">
         <v>732.45</v>
       </c>
-      <c r="I7" t="str">
+      <c r="J7" t="str">
         <v>8.17</v>
       </c>
-      <c r="J7" t="str">
-        <v>45.08</v>
-      </c>
       <c r="K7" t="str">
+        <v>45.08</v>
+      </c>
+      <c r="L7" t="str">
         <v>728.63</v>
       </c>
-      <c r="L7" t="str">
+      <c r="M7" t="str">
         <v>0.72</v>
       </c>
-      <c r="M7" t="str">
+      <c r="N7" t="str">
         <v>723.37</v>
       </c>
-      <c r="N7" t="str">
-        <v>0.10</v>
-      </c>
       <c r="O7" t="str">
+        <v>0.10</v>
+      </c>
+      <c r="P7" t="str">
         <v>1019.83</v>
       </c>
-      <c r="P7" t="str">
+      <c r="Q7" t="str">
         <v>1644.25</v>
       </c>
-      <c r="Q7" t="str">
-        <v>No</v>
-      </c>
       <c r="R7" t="str">
+        <v>No</v>
+      </c>
+      <c r="S7" t="str">
         <v>843.20</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8">
+      <c r="A8" t="str">
+        <v>Scenario 1 - Gradual Increase</v>
+      </c>
+      <c r="B8">
         <v>7</v>
       </c>
-      <c r="B8">
+      <c r="C8">
         <v>3300</v>
       </c>
-      <c r="C8" t="str">
-        <v>150.00</v>
-      </c>
       <c r="D8" t="str">
+        <v>150.00</v>
+      </c>
+      <c r="E8" t="str">
         <v>0.410714</v>
       </c>
-      <c r="E8" t="str">
+      <c r="F8" t="str">
         <v>0.413649</v>
       </c>
-      <c r="F8" t="str">
+      <c r="G8" t="str">
         <v>1365.04</v>
       </c>
-      <c r="G8" t="str">
+      <c r="H8" t="str">
         <v>209.70</v>
       </c>
-      <c r="H8" t="str">
+      <c r="I8" t="str">
         <v>943.72</v>
       </c>
-      <c r="I8" t="str">
+      <c r="J8" t="str">
         <v>10.02</v>
       </c>
-      <c r="J8" t="str">
-        <v>45.08</v>
-      </c>
       <c r="K8" t="str">
+        <v>45.08</v>
+      </c>
+      <c r="L8" t="str">
         <v>938.33</v>
       </c>
-      <c r="L8" t="str">
+      <c r="M8" t="str">
         <v>2.02</v>
       </c>
-      <c r="M8" t="str">
+      <c r="N8" t="str">
         <v>919.38</v>
       </c>
-      <c r="N8" t="str">
-        <v>0.10</v>
-      </c>
       <c r="O8" t="str">
+        <v>0.10</v>
+      </c>
+      <c r="P8" t="str">
         <v>1340.60</v>
       </c>
-      <c r="P8" t="str">
+      <c r="Q8" t="str">
         <v>1882.20</v>
       </c>
-      <c r="Q8" t="str">
-        <v>No</v>
-      </c>
       <c r="R8" t="str">
+        <v>No</v>
+      </c>
+      <c r="S8" t="str">
         <v>1209.97</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9">
+      <c r="A9" t="str">
+        <v>Scenario 1 - Gradual Increase</v>
+      </c>
+      <c r="B9">
         <v>8</v>
       </c>
-      <c r="B9">
+      <c r="C9">
         <v>3300</v>
       </c>
-      <c r="C9" t="str">
-        <v>150.00</v>
-      </c>
       <c r="D9" t="str">
+        <v>150.00</v>
+      </c>
+      <c r="E9" t="str">
         <v>0.456169</v>
       </c>
-      <c r="E9" t="str">
+      <c r="F9" t="str">
         <v>0.459869</v>
       </c>
-      <c r="F9" t="str">
+      <c r="G9" t="str">
         <v>1517.57</v>
       </c>
-      <c r="G9" t="str">
+      <c r="H9" t="str">
         <v>161.43</v>
       </c>
-      <c r="H9" t="str">
+      <c r="I9" t="str">
         <v>1107.00</v>
       </c>
-      <c r="I9" t="str">
+      <c r="J9" t="str">
         <v>6.57</v>
       </c>
-      <c r="J9" t="str">
+      <c r="K9" t="str">
         <v>45.07</v>
       </c>
-      <c r="K9" t="str">
+      <c r="L9" t="str">
         <v>1099.77</v>
       </c>
-      <c r="L9" t="str">
+      <c r="M9" t="str">
         <v>2.02</v>
       </c>
-      <c r="M9" t="str">
+      <c r="N9" t="str">
         <v>1077.55</v>
       </c>
-      <c r="N9" t="str">
-        <v>0.10</v>
-      </c>
       <c r="O9" t="str">
+        <v>0.10</v>
+      </c>
+      <c r="P9" t="str">
         <v>1488.02</v>
       </c>
-      <c r="P9" t="str">
+      <c r="Q9" t="str">
         <v>1985.94</v>
       </c>
-      <c r="Q9" t="str">
-        <v>No</v>
-      </c>
       <c r="R9" t="str">
+        <v>No</v>
+      </c>
+      <c r="S9" t="str">
         <v>1365.56</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10">
+      <c r="A10" t="str">
+        <v>Scenario 1 - Gradual Increase</v>
+      </c>
+      <c r="B10">
         <v>9</v>
       </c>
-      <c r="B10">
+      <c r="C10">
         <v>3300</v>
       </c>
-      <c r="C10" t="str">
-        <v>150.00</v>
-      </c>
       <c r="D10" t="str">
+        <v>150.00</v>
+      </c>
+      <c r="E10" t="str">
         <v>0.501623</v>
       </c>
-      <c r="E10" t="str">
+      <c r="F10" t="str">
         <v>0.506166</v>
       </c>
-      <c r="F10" t="str">
+      <c r="G10" t="str">
         <v>1670.35</v>
       </c>
-      <c r="G10" t="str">
+      <c r="H10" t="str">
         <v>139.55</v>
       </c>
-      <c r="H10" t="str">
+      <c r="I10" t="str">
         <v>1248.63</v>
       </c>
-      <c r="I10" t="str">
+      <c r="J10" t="str">
         <v>5.04</v>
       </c>
-      <c r="J10" t="str">
-        <v>45.08</v>
-      </c>
       <c r="K10" t="str">
+        <v>45.08</v>
+      </c>
+      <c r="L10" t="str">
         <v>1239.32</v>
       </c>
-      <c r="L10" t="str">
+      <c r="M10" t="str">
         <v>2.02</v>
       </c>
-      <c r="M10" t="str">
+      <c r="N10" t="str">
         <v>1214.28</v>
       </c>
-      <c r="N10" t="str">
-        <v>0.10</v>
-      </c>
       <c r="O10" t="str">
+        <v>0.10</v>
+      </c>
+      <c r="P10" t="str">
         <v>1635.90</v>
       </c>
-      <c r="P10" t="str">
+      <c r="Q10" t="str">
         <v>2035.14</v>
       </c>
-      <c r="Q10" t="str">
-        <v>No</v>
-      </c>
       <c r="R10" t="str">
+        <v>No</v>
+      </c>
+      <c r="S10" t="str">
         <v>1500.18</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11">
+      <c r="A11" t="str">
+        <v>Scenario 1 - Gradual Increase</v>
+      </c>
+      <c r="B11">
         <v>10</v>
       </c>
-      <c r="B11">
+      <c r="C11">
         <v>4000</v>
       </c>
-      <c r="C11" t="str">
-        <v>150.00</v>
-      </c>
       <c r="D11" t="str">
+        <v>150.00</v>
+      </c>
+      <c r="E11" t="str">
         <v>0.539123</v>
       </c>
-      <c r="E11" t="str">
+      <c r="F11" t="str">
         <v>0.544572</v>
       </c>
-      <c r="F11" t="str">
+      <c r="G11" t="str">
         <v>2178.29</v>
       </c>
-      <c r="G11" t="str">
+      <c r="H11" t="str">
         <v>289.29</v>
       </c>
-      <c r="H11" t="str">
+      <c r="I11" t="str">
         <v>1540.49</v>
       </c>
-      <c r="I11" t="str">
+      <c r="J11" t="str">
         <v>8.46</v>
       </c>
-      <c r="J11" t="str">
-        <v>45.08</v>
-      </c>
       <c r="K11" t="str">
+        <v>45.08</v>
+      </c>
+      <c r="L11" t="str">
         <v>1528.61</v>
       </c>
-      <c r="L11" t="str">
+      <c r="M11" t="str">
         <v>4.31</v>
       </c>
-      <c r="M11" t="str">
+      <c r="N11" t="str">
         <v>1462.78</v>
       </c>
-      <c r="N11" t="str">
-        <v>0.10</v>
-      </c>
       <c r="O11" t="str">
+        <v>0.10</v>
+      </c>
+      <c r="P11" t="str">
         <v>2100.48</v>
       </c>
-      <c r="P11" t="str">
+      <c r="Q11" t="str">
         <v>2333.76</v>
       </c>
-      <c r="Q11" t="str">
-        <v>No</v>
-      </c>
       <c r="R11" t="str">
+        <v>No</v>
+      </c>
+      <c r="S11" t="str">
         <v>2063.25</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12">
+      <c r="A12" t="str">
+        <v>Scenario 1 - Gradual Increase</v>
+      </c>
+      <c r="B12">
         <v>11</v>
       </c>
-      <c r="B12">
+      <c r="C12">
         <v>4000</v>
       </c>
-      <c r="C12" t="str">
-        <v>150.00</v>
-      </c>
       <c r="D12" t="str">
+        <v>150.00</v>
+      </c>
+      <c r="E12" t="str">
         <v>0.576623</v>
       </c>
-      <c r="E12" t="str">
+      <c r="F12" t="str">
         <v>0.583042</v>
       </c>
-      <c r="F12" t="str">
+      <c r="G12" t="str">
         <v>2332.17</v>
       </c>
-      <c r="G12" t="str">
+      <c r="H12" t="str">
         <v>196.87</v>
       </c>
-      <c r="H12" t="str">
+      <c r="I12" t="str">
         <v>1740.25</v>
       </c>
-      <c r="I12" t="str">
+      <c r="J12" t="str">
         <v>5.10</v>
       </c>
-      <c r="J12" t="str">
+      <c r="K12" t="str">
         <v>45.07</v>
       </c>
-      <c r="K12" t="str">
+      <c r="L12" t="str">
         <v>1725.48</v>
       </c>
-      <c r="L12" t="str">
+      <c r="M12" t="str">
         <v>4.31</v>
       </c>
-      <c r="M12" t="str">
+      <c r="N12" t="str">
         <v>1651.16</v>
       </c>
-      <c r="N12" t="str">
-        <v>0.10</v>
-      </c>
       <c r="O12" t="str">
+        <v>0.10</v>
+      </c>
+      <c r="P12" t="str">
         <v>2242.98</v>
       </c>
-      <c r="P12" t="str">
+      <c r="Q12" t="str">
         <v>2462.44</v>
       </c>
-      <c r="Q12" t="str">
-        <v>No</v>
-      </c>
       <c r="R12" t="str">
+        <v>No</v>
+      </c>
+      <c r="S12" t="str">
         <v>2244.14</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13">
+      <c r="A13" t="str">
+        <v>Scenario 1 - Gradual Increase</v>
+      </c>
+      <c r="B13">
         <v>12</v>
       </c>
-      <c r="B13">
+      <c r="C13">
         <v>4000</v>
       </c>
-      <c r="C13" t="str">
-        <v>150.00</v>
-      </c>
       <c r="D13" t="str">
+        <v>150.00</v>
+      </c>
+      <c r="E13" t="str">
         <v>0.614123</v>
       </c>
-      <c r="E13" t="str">
+      <c r="F13" t="str">
         <v>0.621576</v>
       </c>
-      <c r="F13" t="str">
+      <c r="G13" t="str">
         <v>2486.30</v>
       </c>
-      <c r="G13" t="str">
+      <c r="H13" t="str">
         <v>155.06</v>
       </c>
-      <c r="H13" t="str">
+      <c r="I13" t="str">
         <v>1898.46</v>
       </c>
-      <c r="I13" t="str">
+      <c r="J13" t="str">
         <v>3.68</v>
       </c>
-      <c r="J13" t="str">
-        <v>45.08</v>
-      </c>
       <c r="K13" t="str">
+        <v>45.08</v>
+      </c>
+      <c r="L13" t="str">
         <v>1880.54</v>
       </c>
-      <c r="L13" t="str">
+      <c r="M13" t="str">
         <v>4.31</v>
       </c>
-      <c r="M13" t="str">
+      <c r="N13" t="str">
         <v>1799.54</v>
       </c>
-      <c r="N13" t="str">
-        <v>0.10</v>
-      </c>
       <c r="O13" t="str">
+        <v>0.10</v>
+      </c>
+      <c r="P13" t="str">
         <v>2387.28</v>
       </c>
-      <c r="P13" t="str">
+      <c r="Q13" t="str">
         <v>2519.77</v>
       </c>
-      <c r="Q13" t="str">
-        <v>No</v>
-      </c>
       <c r="R13" t="str">
+        <v>No</v>
+      </c>
+      <c r="S13" t="str">
         <v>2386.82</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:R13"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:S13"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:R13"/>
+  <dimension ref="A1:S13"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
+        <v>Scenario</v>
+      </c>
+      <c r="B1" t="str">
         <v>Month</v>
       </c>
-      <c r="B1" t="str">
+      <c r="C1" t="str">
         <v>ETH Price at Deposit ($/ETH)</v>
       </c>
-      <c r="C1" t="str">
+      <c r="D1" t="str">
         <v>Deposit Amount ($)</v>
       </c>
-      <c r="D1" t="str">
+      <c r="E1" t="str">
         <v>Total ETH Held Without Interest (ETH)</v>
       </c>
-      <c r="E1" t="str">
+      <c r="F1" t="str">
         <v>Total ETH Held With Interest (ETH)</v>
       </c>
-      <c r="F1" t="str">
+      <c r="G1" t="str">
         <v>Total ETH Value (USD)</v>
       </c>
-      <c r="G1" t="str">
+      <c r="H1" t="str">
         <v>Borrowed Amount (This Month, $)</v>
       </c>
-      <c r="H1" t="str">
+      <c r="I1" t="str">
         <v>Total Borrowed with Interest ($)</v>
       </c>
-      <c r="I1" t="str">
+      <c r="J1" t="str">
         <v>Borrow Rate (%)</v>
       </c>
-      <c r="J1" t="str">
+      <c r="K1" t="str">
         <v>LTV (%)</v>
       </c>
-      <c r="K1" t="str">
+      <c r="L1" t="str">
         <v>LP Growth ($)</v>
       </c>
-      <c r="L1" t="str">
+      <c r="M1" t="str">
         <v>Impermanent Loss (%)</v>
       </c>
-      <c r="M1" t="str">
+      <c r="N1" t="str">
         <v>LP Value After IL ($)</v>
       </c>
-      <c r="N1" t="str">
+      <c r="O1" t="str">
         <v>Gas Fee (Base Chain) ($)</v>
       </c>
-      <c r="O1" t="str">
+      <c r="P1" t="str">
         <v>Net Capital ($)</v>
       </c>
-      <c r="P1" t="str">
+      <c r="Q1" t="str">
         <v>ETH Liquidation Price ($)</v>
       </c>
-      <c r="Q1" t="str">
+      <c r="R1" t="str">
         <v>Liquidated?</v>
       </c>
-      <c r="R1" t="str">
+      <c r="S1" t="str">
         <v>Profit ($)</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2">
+      <c r="A2" t="str">
+        <v>Scenario 2 - Gradual Decrease</v>
+      </c>
+      <c r="B2">
         <v>1</v>
       </c>
-      <c r="B2">
+      <c r="C2">
         <v>4000</v>
       </c>
-      <c r="C2" t="str">
-        <v>150.00</v>
-      </c>
       <c r="D2" t="str">
+        <v>150.00</v>
+      </c>
+      <c r="E2" t="str">
         <v>0.037500</v>
       </c>
-      <c r="E2" t="str">
+      <c r="F2" t="str">
         <v>0.037562</v>
       </c>
-      <c r="F2" t="str">
+      <c r="G2" t="str">
         <v>150.25</v>
       </c>
-      <c r="G2" t="str">
+      <c r="H2" t="str">
         <v>67.61</v>
       </c>
-      <c r="H2" t="str">
+      <c r="I2" t="str">
         <v>67.73</v>
       </c>
-      <c r="I2" t="str">
+      <c r="J2" t="str">
         <v>45.00</v>
       </c>
-      <c r="J2" t="str">
-        <v>45.08</v>
-      </c>
       <c r="K2" t="str">
+        <v>45.08</v>
+      </c>
+      <c r="L2" t="str">
         <v>67.61</v>
       </c>
-      <c r="L2" t="str">
+      <c r="M2" t="str">
         <v>4.31</v>
       </c>
-      <c r="M2" t="str">
+      <c r="N2" t="str">
         <v>64.70</v>
       </c>
-      <c r="N2" t="str">
-        <v>0.10</v>
-      </c>
       <c r="O2" t="str">
+        <v>0.10</v>
+      </c>
+      <c r="P2" t="str">
         <v>147.13</v>
       </c>
-      <c r="P2" t="str">
+      <c r="Q2" t="str">
         <v>1487.48</v>
       </c>
-      <c r="Q2" t="str">
-        <v>No</v>
-      </c>
       <c r="R2" t="str">
+        <v>No</v>
+      </c>
+      <c r="S2" t="str">
         <v>61.83</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3">
+      <c r="A3" t="str">
+        <v>Scenario 2 - Gradual Decrease</v>
+      </c>
+      <c r="B3">
         <v>2</v>
       </c>
-      <c r="B3">
+      <c r="C3">
         <v>4000</v>
       </c>
-      <c r="C3" t="str">
-        <v>150.00</v>
-      </c>
       <c r="D3" t="str">
+        <v>150.00</v>
+      </c>
+      <c r="E3" t="str">
         <v>0.075000</v>
       </c>
-      <c r="E3" t="str">
+      <c r="F3" t="str">
         <v>0.075188</v>
       </c>
-      <c r="F3" t="str">
+      <c r="G3" t="str">
         <v>300.75</v>
       </c>
-      <c r="G3" t="str">
+      <c r="H3" t="str">
         <v>98.04</v>
       </c>
-      <c r="H3" t="str">
+      <c r="I3" t="str">
         <v>166.04</v>
       </c>
-      <c r="I3" t="str">
+      <c r="J3" t="str">
         <v>26.61</v>
       </c>
-      <c r="J3" t="str">
-        <v>45.08</v>
-      </c>
       <c r="K3" t="str">
+        <v>45.08</v>
+      </c>
+      <c r="L3" t="str">
         <v>165.65</v>
       </c>
-      <c r="L3" t="str">
+      <c r="M3" t="str">
         <v>4.31</v>
       </c>
-      <c r="M3" t="str">
+      <c r="N3" t="str">
         <v>158.52</v>
       </c>
-      <c r="N3" t="str">
-        <v>0.10</v>
-      </c>
       <c r="O3" t="str">
+        <v>0.10</v>
+      </c>
+      <c r="P3" t="str">
         <v>293.13</v>
       </c>
-      <c r="P3" t="str">
+      <c r="Q3" t="str">
         <v>1821.88</v>
       </c>
-      <c r="Q3" t="str">
-        <v>No</v>
-      </c>
       <c r="R3" t="str">
+        <v>No</v>
+      </c>
+      <c r="S3" t="str">
         <v>151.64</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4">
+      <c r="A4" t="str">
+        <v>Scenario 2 - Gradual Decrease</v>
+      </c>
+      <c r="B4">
         <v>3</v>
       </c>
-      <c r="B4">
+      <c r="C4">
         <v>4000</v>
       </c>
-      <c r="C4" t="str">
-        <v>150.00</v>
-      </c>
       <c r="D4" t="str">
+        <v>150.00</v>
+      </c>
+      <c r="E4" t="str">
         <v>0.112500</v>
       </c>
-      <c r="E4" t="str">
+      <c r="F4" t="str">
         <v>0.112875</v>
       </c>
-      <c r="F4" t="str">
+      <c r="G4" t="str">
         <v>451.50</v>
       </c>
-      <c r="G4" t="str">
+      <c r="H4" t="str">
         <v>111.68</v>
       </c>
-      <c r="H4" t="str">
+      <c r="I4" t="str">
         <v>278.18</v>
       </c>
-      <c r="I4" t="str">
+      <c r="J4" t="str">
         <v>18.10</v>
       </c>
-      <c r="J4" t="str">
-        <v>45.08</v>
-      </c>
       <c r="K4" t="str">
+        <v>45.08</v>
+      </c>
+      <c r="L4" t="str">
         <v>277.33</v>
       </c>
-      <c r="L4" t="str">
+      <c r="M4" t="str">
         <v>4.31</v>
       </c>
-      <c r="M4" t="str">
+      <c r="N4" t="str">
         <v>265.38</v>
       </c>
-      <c r="N4" t="str">
-        <v>0.10</v>
-      </c>
       <c r="O4" t="str">
+        <v>0.10</v>
+      </c>
+      <c r="P4" t="str">
         <v>438.60</v>
       </c>
-      <c r="P4" t="str">
+      <c r="Q4" t="str">
         <v>2033.21</v>
       </c>
-      <c r="Q4" t="str">
-        <v>No</v>
-      </c>
       <c r="R4" t="str">
+        <v>No</v>
+      </c>
+      <c r="S4" t="str">
         <v>253.99</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5">
+      <c r="A5" t="str">
+        <v>Scenario 2 - Gradual Decrease</v>
+      </c>
+      <c r="B5">
         <v>4</v>
       </c>
-      <c r="B5">
+      <c r="C5">
         <v>3300</v>
       </c>
-      <c r="C5" t="str">
-        <v>150.00</v>
-      </c>
       <c r="D5" t="str">
+        <v>150.00</v>
+      </c>
+      <c r="E5" t="str">
         <v>0.157955</v>
       </c>
-      <c r="E5" t="str">
+      <c r="F5" t="str">
         <v>0.158594</v>
       </c>
-      <c r="F5" t="str">
+      <c r="G5" t="str">
         <v>523.36</v>
       </c>
-      <c r="G5" t="str">
+      <c r="H5" t="str">
         <v>82.13</v>
       </c>
-      <c r="H5" t="str">
+      <c r="I5" t="str">
         <v>360.91</v>
       </c>
-      <c r="I5" t="str">
+      <c r="J5" t="str">
         <v>10.26</v>
       </c>
-      <c r="J5" t="str">
-        <v>45.08</v>
-      </c>
       <c r="K5" t="str">
+        <v>45.08</v>
+      </c>
+      <c r="L5" t="str">
         <v>359.46</v>
       </c>
-      <c r="L5" t="str">
+      <c r="M5" t="str">
         <v>2.02</v>
       </c>
-      <c r="M5" t="str">
+      <c r="N5" t="str">
         <v>352.20</v>
       </c>
-      <c r="N5" t="str">
-        <v>0.10</v>
-      </c>
       <c r="O5" t="str">
+        <v>0.10</v>
+      </c>
+      <c r="P5" t="str">
         <v>514.54</v>
       </c>
-      <c r="P5" t="str">
+      <c r="Q5" t="str">
         <v>1877.45</v>
       </c>
-      <c r="Q5" t="str">
-        <v>No</v>
-      </c>
       <c r="R5" t="str">
+        <v>No</v>
+      </c>
+      <c r="S5" t="str">
         <v>266.74</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6">
+      <c r="A6" t="str">
+        <v>Scenario 2 - Gradual Decrease</v>
+      </c>
+      <c r="B6">
         <v>5</v>
       </c>
-      <c r="B6">
+      <c r="C6">
         <v>3300</v>
       </c>
-      <c r="C6" t="str">
-        <v>150.00</v>
-      </c>
       <c r="D6" t="str">
+        <v>150.00</v>
+      </c>
+      <c r="E6" t="str">
         <v>0.203409</v>
       </c>
-      <c r="E6" t="str">
+      <c r="F6" t="str">
         <v>0.204388</v>
       </c>
-      <c r="F6" t="str">
+      <c r="G6" t="str">
         <v>674.48</v>
       </c>
-      <c r="G6" t="str">
+      <c r="H6" t="str">
         <v>104.36</v>
       </c>
-      <c r="H6" t="str">
+      <c r="I6" t="str">
         <v>466.05</v>
       </c>
-      <c r="I6" t="str">
+      <c r="J6" t="str">
         <v>10.09</v>
       </c>
-      <c r="J6" t="str">
-        <v>45.08</v>
-      </c>
       <c r="K6" t="str">
+        <v>45.08</v>
+      </c>
+      <c r="L6" t="str">
         <v>463.82</v>
       </c>
-      <c r="L6" t="str">
+      <c r="M6" t="str">
         <v>2.02</v>
       </c>
-      <c r="M6" t="str">
+      <c r="N6" t="str">
         <v>454.45</v>
       </c>
-      <c r="N6" t="str">
-        <v>0.10</v>
-      </c>
       <c r="O6" t="str">
+        <v>0.10</v>
+      </c>
+      <c r="P6" t="str">
         <v>662.78</v>
       </c>
-      <c r="P6" t="str">
+      <c r="Q6" t="str">
         <v>1881.17</v>
       </c>
-      <c r="Q6" t="str">
-        <v>No</v>
-      </c>
       <c r="R6" t="str">
+        <v>No</v>
+      </c>
+      <c r="S6" t="str">
         <v>367.23</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7">
+      <c r="A7" t="str">
+        <v>Scenario 2 - Gradual Decrease</v>
+      </c>
+      <c r="B7">
         <v>6</v>
       </c>
-      <c r="B7">
+      <c r="C7">
         <v>3300</v>
       </c>
-      <c r="C7" t="str">
-        <v>150.00</v>
-      </c>
       <c r="D7" t="str">
+        <v>150.00</v>
+      </c>
+      <c r="E7" t="str">
         <v>0.248864</v>
       </c>
-      <c r="E7" t="str">
+      <c r="F7" t="str">
         <v>0.250259</v>
       </c>
-      <c r="F7" t="str">
+      <c r="G7" t="str">
         <v>825.86</v>
       </c>
-      <c r="G7" t="str">
+      <c r="H7" t="str">
         <v>114.31</v>
       </c>
-      <c r="H7" t="str">
+      <c r="I7" t="str">
         <v>581.32</v>
       </c>
-      <c r="I7" t="str">
+      <c r="J7" t="str">
         <v>8.86</v>
       </c>
-      <c r="J7" t="str">
-        <v>45.08</v>
-      </c>
       <c r="K7" t="str">
+        <v>45.08</v>
+      </c>
+      <c r="L7" t="str">
         <v>578.13</v>
       </c>
-      <c r="L7" t="str">
+      <c r="M7" t="str">
         <v>2.02</v>
       </c>
-      <c r="M7" t="str">
+      <c r="N7" t="str">
         <v>566.45</v>
       </c>
-      <c r="N7" t="str">
-        <v>0.10</v>
-      </c>
       <c r="O7" t="str">
+        <v>0.10</v>
+      </c>
+      <c r="P7" t="str">
         <v>810.88</v>
       </c>
-      <c r="P7" t="str">
+      <c r="Q7" t="str">
         <v>1916.37</v>
       </c>
-      <c r="Q7" t="str">
-        <v>No</v>
-      </c>
       <c r="R7" t="str">
+        <v>No</v>
+      </c>
+      <c r="S7" t="str">
         <v>477.33</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8">
+      <c r="A8" t="str">
+        <v>Scenario 2 - Gradual Decrease</v>
+      </c>
+      <c r="B8">
         <v>7</v>
       </c>
-      <c r="B8">
+      <c r="C8">
         <v>2800</v>
       </c>
-      <c r="C8" t="str">
-        <v>150.00</v>
-      </c>
       <c r="D8" t="str">
+        <v>150.00</v>
+      </c>
+      <c r="E8" t="str">
         <v>0.302435</v>
       </c>
-      <c r="E8" t="str">
+      <c r="F8" t="str">
         <v>0.304337</v>
       </c>
-      <c r="F8" t="str">
+      <c r="G8" t="str">
         <v>852.14</v>
       </c>
-      <c r="G8" t="str">
+      <c r="H8" t="str">
         <v>62.30</v>
       </c>
-      <c r="H8" t="str">
+      <c r="I8" t="str">
         <v>644.69</v>
       </c>
-      <c r="I8" t="str">
+      <c r="J8" t="str">
         <v>4.36</v>
       </c>
-      <c r="J8" t="str">
-        <v>45.08</v>
-      </c>
       <c r="K8" t="str">
+        <v>45.08</v>
+      </c>
+      <c r="L8" t="str">
         <v>640.43</v>
       </c>
-      <c r="L8" t="str">
+      <c r="M8" t="str">
         <v>0.72</v>
       </c>
-      <c r="M8" t="str">
+      <c r="N8" t="str">
         <v>635.80</v>
       </c>
-      <c r="N8" t="str">
-        <v>0.10</v>
-      </c>
       <c r="O8" t="str">
+        <v>0.10</v>
+      </c>
+      <c r="P8" t="str">
         <v>843.15</v>
       </c>
-      <c r="P8" t="str">
+      <c r="Q8" t="str">
         <v>1747.64</v>
       </c>
-      <c r="Q8" t="str">
-        <v>No</v>
-      </c>
       <c r="R8" t="str">
+        <v>No</v>
+      </c>
+      <c r="S8" t="str">
         <v>428.95</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9">
+      <c r="A9" t="str">
+        <v>Scenario 2 - Gradual Decrease</v>
+      </c>
+      <c r="B9">
         <v>8</v>
       </c>
-      <c r="B9">
+      <c r="C9">
         <v>2800</v>
       </c>
-      <c r="C9" t="str">
-        <v>150.00</v>
-      </c>
       <c r="D9" t="str">
+        <v>150.00</v>
+      </c>
+      <c r="E9" t="str">
         <v>0.356006</v>
       </c>
-      <c r="E9" t="str">
+      <c r="F9" t="str">
         <v>0.358505</v>
       </c>
-      <c r="F9" t="str">
+      <c r="G9" t="str">
         <v>1003.81</v>
       </c>
-      <c r="G9" t="str">
+      <c r="H9" t="str">
         <v>95.21</v>
       </c>
-      <c r="H9" t="str">
+      <c r="I9" t="str">
         <v>741.14</v>
       </c>
-      <c r="I9" t="str">
+      <c r="J9" t="str">
         <v>5.79</v>
       </c>
-      <c r="J9" t="str">
+      <c r="K9" t="str">
         <v>45.07</v>
       </c>
-      <c r="K9" t="str">
+      <c r="L9" t="str">
         <v>735.64</v>
       </c>
-      <c r="L9" t="str">
+      <c r="M9" t="str">
         <v>0.72</v>
       </c>
-      <c r="M9" t="str">
+      <c r="N9" t="str">
         <v>730.33</v>
       </c>
-      <c r="N9" t="str">
-        <v>0.10</v>
-      </c>
       <c r="O9" t="str">
+        <v>0.10</v>
+      </c>
+      <c r="P9" t="str">
         <v>992.90</v>
       </c>
-      <c r="P9" t="str">
+      <c r="Q9" t="str">
         <v>1705.53</v>
       </c>
-      <c r="Q9" t="str">
-        <v>No</v>
-      </c>
       <c r="R9" t="str">
+        <v>No</v>
+      </c>
+      <c r="S9" t="str">
         <v>523.22</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10">
+      <c r="A10" t="str">
+        <v>Scenario 2 - Gradual Decrease</v>
+      </c>
+      <c r="B10">
         <v>9</v>
       </c>
-      <c r="B10">
+      <c r="C10">
         <v>2800</v>
       </c>
-      <c r="C10" t="str">
-        <v>150.00</v>
-      </c>
       <c r="D10" t="str">
+        <v>150.00</v>
+      </c>
+      <c r="E10" t="str">
         <v>0.409578</v>
       </c>
-      <c r="E10" t="str">
+      <c r="F10" t="str">
         <v>0.412763</v>
       </c>
-      <c r="F10" t="str">
+      <c r="G10" t="str">
         <v>1155.74</v>
       </c>
-      <c r="G10" t="str">
+      <c r="H10" t="str">
         <v>109.98</v>
       </c>
-      <c r="H10" t="str">
+      <c r="I10" t="str">
         <v>852.54</v>
       </c>
-      <c r="I10" t="str">
+      <c r="J10" t="str">
         <v>5.81</v>
       </c>
-      <c r="J10" t="str">
-        <v>45.08</v>
-      </c>
       <c r="K10" t="str">
+        <v>45.08</v>
+      </c>
+      <c r="L10" t="str">
         <v>845.62</v>
       </c>
-      <c r="L10" t="str">
+      <c r="M10" t="str">
         <v>0.72</v>
       </c>
-      <c r="M10" t="str">
+      <c r="N10" t="str">
         <v>839.51</v>
       </c>
-      <c r="N10" t="str">
-        <v>0.10</v>
-      </c>
       <c r="O10" t="str">
+        <v>0.10</v>
+      </c>
+      <c r="P10" t="str">
         <v>1142.61</v>
       </c>
-      <c r="P10" t="str">
+      <c r="Q10" t="str">
         <v>1703.99</v>
       </c>
-      <c r="Q10" t="str">
-        <v>No</v>
-      </c>
       <c r="R10" t="str">
+        <v>No</v>
+      </c>
+      <c r="S10" t="str">
         <v>632.12</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11">
+      <c r="A11" t="str">
+        <v>Scenario 2 - Gradual Decrease</v>
+      </c>
+      <c r="B11">
         <v>10</v>
       </c>
-      <c r="B11">
+      <c r="C11">
         <v>2200</v>
       </c>
-      <c r="C11" t="str">
-        <v>150.00</v>
-      </c>
       <c r="D11" t="str">
+        <v>150.00</v>
+      </c>
+      <c r="E11" t="str">
         <v>0.477760</v>
       </c>
-      <c r="E11" t="str">
+      <c r="F11" t="str">
         <v>0.481747</v>
       </c>
-      <c r="F11" t="str">
+      <c r="G11" t="str">
         <v>1059.84</v>
       </c>
-      <c r="G11" t="str">
+      <c r="H11" t="str">
         <v>4.92</v>
       </c>
-      <c r="H11" t="str">
+      <c r="I11" t="str">
         <v>858.89</v>
       </c>
-      <c r="I11" t="str">
+      <c r="J11" t="str">
         <v>0.26</v>
       </c>
-      <c r="J11" t="str">
-        <v>45.08</v>
-      </c>
       <c r="K11" t="str">
+        <v>45.08</v>
+      </c>
+      <c r="L11" t="str">
         <v>850.54</v>
       </c>
-      <c r="L11" t="str">
+      <c r="M11" t="str">
         <v>0.00</v>
       </c>
-      <c r="M11" t="str">
+      <c r="N11" t="str">
         <v>850.54</v>
       </c>
-      <c r="N11" t="str">
-        <v>0.10</v>
-      </c>
       <c r="O11" t="str">
+        <v>0.10</v>
+      </c>
+      <c r="P11" t="str">
         <v>1051.39</v>
       </c>
-      <c r="P11" t="str">
+      <c r="Q11" t="str">
         <v>1470.86</v>
       </c>
-      <c r="Q11" t="str">
-        <v>No</v>
-      </c>
       <c r="R11" t="str">
+        <v>No</v>
+      </c>
+      <c r="S11" t="str">
         <v>401.93</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12">
+      <c r="A12" t="str">
+        <v>Scenario 2 - Gradual Decrease</v>
+      </c>
+      <c r="B12">
         <v>11</v>
       </c>
-      <c r="B12">
+      <c r="C12">
         <v>2200</v>
       </c>
-      <c r="C12" t="str">
-        <v>150.00</v>
-      </c>
       <c r="D12" t="str">
+        <v>150.00</v>
+      </c>
+      <c r="E12" t="str">
         <v>0.545942</v>
       </c>
-      <c r="E12" t="str">
+      <c r="F12" t="str">
         <v>0.550845</v>
       </c>
-      <c r="F12" t="str">
+      <c r="G12" t="str">
         <v>1211.86</v>
       </c>
-      <c r="G12" t="str">
+      <c r="H12" t="str">
         <v>69.19</v>
       </c>
-      <c r="H12" t="str">
+      <c r="I12" t="str">
         <v>929.63</v>
       </c>
-      <c r="I12" t="str">
+      <c r="J12" t="str">
         <v>3.35</v>
       </c>
-      <c r="J12" t="str">
+      <c r="K12" t="str">
         <v>45.07</v>
       </c>
-      <c r="K12" t="str">
+      <c r="L12" t="str">
         <v>919.73</v>
       </c>
-      <c r="L12" t="str">
+      <c r="M12" t="str">
         <v>0.00</v>
       </c>
-      <c r="M12" t="str">
+      <c r="N12" t="str">
         <v>919.73</v>
       </c>
-      <c r="N12" t="str">
-        <v>0.10</v>
-      </c>
       <c r="O12" t="str">
+        <v>0.10</v>
+      </c>
+      <c r="P12" t="str">
         <v>1201.86</v>
       </c>
-      <c r="P12" t="str">
+      <c r="Q12" t="str">
         <v>1392.30</v>
       </c>
-      <c r="Q12" t="str">
-        <v>No</v>
-      </c>
       <c r="R12" t="str">
+        <v>No</v>
+      </c>
+      <c r="S12" t="str">
         <v>471.59</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13">
+      <c r="A13" t="str">
+        <v>Scenario 2 - Gradual Decrease</v>
+      </c>
+      <c r="B13">
         <v>12</v>
       </c>
-      <c r="B13">
+      <c r="C13">
         <v>2200</v>
       </c>
-      <c r="C13" t="str">
-        <v>150.00</v>
-      </c>
       <c r="D13" t="str">
+        <v>150.00</v>
+      </c>
+      <c r="E13" t="str">
         <v>0.614123</v>
       </c>
-      <c r="E13" t="str">
+      <c r="F13" t="str">
         <v>0.620059</v>
       </c>
-      <c r="F13" t="str">
+      <c r="G13" t="str">
         <v>1364.13</v>
       </c>
-      <c r="G13" t="str">
+      <c r="H13" t="str">
         <v>98.11</v>
       </c>
-      <c r="H13" t="str">
+      <c r="I13" t="str">
         <v>1029.45</v>
       </c>
-      <c r="I13" t="str">
+      <c r="J13" t="str">
         <v>4.30</v>
       </c>
-      <c r="J13" t="str">
-        <v>45.08</v>
-      </c>
       <c r="K13" t="str">
+        <v>45.08</v>
+      </c>
+      <c r="L13" t="str">
         <v>1017.84</v>
       </c>
-      <c r="L13" t="str">
+      <c r="M13" t="str">
         <v>0.00</v>
       </c>
-      <c r="M13" t="str">
+      <c r="N13" t="str">
         <v>1017.84</v>
       </c>
-      <c r="N13" t="str">
-        <v>0.10</v>
-      </c>
       <c r="O13" t="str">
+        <v>0.10</v>
+      </c>
+      <c r="P13" t="str">
         <v>1352.42</v>
       </c>
-      <c r="P13" t="str">
+      <c r="Q13" t="str">
         <v>1369.70</v>
       </c>
-      <c r="Q13" t="str">
-        <v>No</v>
-      </c>
       <c r="R13" t="str">
+        <v>No</v>
+      </c>
+      <c r="S13" t="str">
         <v>570.26</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:R13"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:S13"/>
+  </ignoredErrors>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:S25"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>Scenario</v>
+      </c>
+      <c r="B1" t="str">
+        <v>Month</v>
+      </c>
+      <c r="C1" t="str">
+        <v>ETH Price at Deposit ($/ETH)</v>
+      </c>
+      <c r="D1" t="str">
+        <v>Deposit Amount ($)</v>
+      </c>
+      <c r="E1" t="str">
+        <v>Total ETH Held Without Interest (ETH)</v>
+      </c>
+      <c r="F1" t="str">
+        <v>Total ETH Held With Interest (ETH)</v>
+      </c>
+      <c r="G1" t="str">
+        <v>Total ETH Value (USD)</v>
+      </c>
+      <c r="H1" t="str">
+        <v>Borrowed Amount (This Month, $)</v>
+      </c>
+      <c r="I1" t="str">
+        <v>Total Borrowed with Interest ($)</v>
+      </c>
+      <c r="J1" t="str">
+        <v>Borrow Rate (%)</v>
+      </c>
+      <c r="K1" t="str">
+        <v>LTV (%)</v>
+      </c>
+      <c r="L1" t="str">
+        <v>LP Growth ($)</v>
+      </c>
+      <c r="M1" t="str">
+        <v>Impermanent Loss (%)</v>
+      </c>
+      <c r="N1" t="str">
+        <v>LP Value After IL ($)</v>
+      </c>
+      <c r="O1" t="str">
+        <v>Gas Fee (Base Chain) ($)</v>
+      </c>
+      <c r="P1" t="str">
+        <v>Net Capital ($)</v>
+      </c>
+      <c r="Q1" t="str">
+        <v>ETH Liquidation Price ($)</v>
+      </c>
+      <c r="R1" t="str">
+        <v>Liquidated?</v>
+      </c>
+      <c r="S1" t="str">
+        <v>Profit ($)</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>Scenario 1 - Gradual Increase</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>2200</v>
+      </c>
+      <c r="D2" t="str">
+        <v>150.00</v>
+      </c>
+      <c r="E2" t="str">
+        <v>0.068182</v>
+      </c>
+      <c r="F2" t="str">
+        <v>0.068295</v>
+      </c>
+      <c r="G2" t="str">
+        <v>150.25</v>
+      </c>
+      <c r="H2" t="str">
+        <v>67.61</v>
+      </c>
+      <c r="I2" t="str">
+        <v>67.73</v>
+      </c>
+      <c r="J2" t="str">
+        <v>45.00</v>
+      </c>
+      <c r="K2" t="str">
+        <v>45.08</v>
+      </c>
+      <c r="L2" t="str">
+        <v>67.61</v>
+      </c>
+      <c r="M2" t="str">
+        <v>0.00</v>
+      </c>
+      <c r="N2" t="str">
+        <v>67.61</v>
+      </c>
+      <c r="O2" t="str">
+        <v>0.10</v>
+      </c>
+      <c r="P2" t="str">
+        <v>150.04</v>
+      </c>
+      <c r="Q2" t="str">
+        <v>818.11</v>
+      </c>
+      <c r="R2" t="str">
+        <v>No</v>
+      </c>
+      <c r="S2" t="str">
+        <v>67.65</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>Scenario 1 - Gradual Increase</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>2200</v>
+      </c>
+      <c r="D3" t="str">
+        <v>150.00</v>
+      </c>
+      <c r="E3" t="str">
+        <v>0.136364</v>
+      </c>
+      <c r="F3" t="str">
+        <v>0.136705</v>
+      </c>
+      <c r="G3" t="str">
+        <v>300.75</v>
+      </c>
+      <c r="H3" t="str">
+        <v>98.04</v>
+      </c>
+      <c r="I3" t="str">
+        <v>166.04</v>
+      </c>
+      <c r="J3" t="str">
+        <v>26.61</v>
+      </c>
+      <c r="K3" t="str">
+        <v>45.08</v>
+      </c>
+      <c r="L3" t="str">
+        <v>165.65</v>
+      </c>
+      <c r="M3" t="str">
+        <v>0.00</v>
+      </c>
+      <c r="N3" t="str">
+        <v>165.65</v>
+      </c>
+      <c r="O3" t="str">
+        <v>0.10</v>
+      </c>
+      <c r="P3" t="str">
+        <v>300.26</v>
+      </c>
+      <c r="Q3" t="str">
+        <v>1002.03</v>
+      </c>
+      <c r="R3" t="str">
+        <v>No</v>
+      </c>
+      <c r="S3" t="str">
+        <v>165.91</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>Scenario 1 - Gradual Increase</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <v>2200</v>
+      </c>
+      <c r="D4" t="str">
+        <v>150.00</v>
+      </c>
+      <c r="E4" t="str">
+        <v>0.204545</v>
+      </c>
+      <c r="F4" t="str">
+        <v>0.205228</v>
+      </c>
+      <c r="G4" t="str">
+        <v>451.50</v>
+      </c>
+      <c r="H4" t="str">
+        <v>111.68</v>
+      </c>
+      <c r="I4" t="str">
+        <v>278.18</v>
+      </c>
+      <c r="J4" t="str">
+        <v>18.10</v>
+      </c>
+      <c r="K4" t="str">
+        <v>45.08</v>
+      </c>
+      <c r="L4" t="str">
+        <v>277.33</v>
+      </c>
+      <c r="M4" t="str">
+        <v>0.00</v>
+      </c>
+      <c r="N4" t="str">
+        <v>277.33</v>
+      </c>
+      <c r="O4" t="str">
+        <v>0.10</v>
+      </c>
+      <c r="P4" t="str">
+        <v>450.55</v>
+      </c>
+      <c r="Q4" t="str">
+        <v>1118.27</v>
+      </c>
+      <c r="R4" t="str">
+        <v>No</v>
+      </c>
+      <c r="S4" t="str">
+        <v>277.88</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v>Scenario 1 - Gradual Increase</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5">
+        <v>2800</v>
+      </c>
+      <c r="D5" t="str">
+        <v>150.00</v>
+      </c>
+      <c r="E5" t="str">
+        <v>0.258117</v>
+      </c>
+      <c r="F5" t="str">
+        <v>0.259231</v>
+      </c>
+      <c r="G5" t="str">
+        <v>725.85</v>
+      </c>
+      <c r="H5" t="str">
+        <v>173.25</v>
+      </c>
+      <c r="I5" t="str">
+        <v>452.18</v>
+      </c>
+      <c r="J5" t="str">
+        <v>17.27</v>
+      </c>
+      <c r="K5" t="str">
+        <v>45.08</v>
+      </c>
+      <c r="L5" t="str">
+        <v>450.58</v>
+      </c>
+      <c r="M5" t="str">
+        <v>0.72</v>
+      </c>
+      <c r="N5" t="str">
+        <v>447.32</v>
+      </c>
+      <c r="O5" t="str">
+        <v>0.10</v>
+      </c>
+      <c r="P5" t="str">
+        <v>720.89</v>
+      </c>
+      <c r="Q5" t="str">
+        <v>1439.06</v>
+      </c>
+      <c r="R5" t="str">
+        <v>No</v>
+      </c>
+      <c r="S5" t="str">
+        <v>568.21</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="str">
+        <v>Scenario 1 - Gradual Increase</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="C6">
+        <v>2800</v>
+      </c>
+      <c r="D6" t="str">
+        <v>150.00</v>
+      </c>
+      <c r="E6" t="str">
+        <v>0.311688</v>
+      </c>
+      <c r="F6" t="str">
+        <v>0.313324</v>
+      </c>
+      <c r="G6" t="str">
+        <v>877.31</v>
+      </c>
+      <c r="H6" t="str">
+        <v>145.37</v>
+      </c>
+      <c r="I6" t="str">
+        <v>598.54</v>
+      </c>
+      <c r="J6" t="str">
+        <v>10.95</v>
+      </c>
+      <c r="K6" t="str">
+        <v>45.07</v>
+      </c>
+      <c r="L6" t="str">
+        <v>595.94</v>
+      </c>
+      <c r="M6" t="str">
+        <v>0.72</v>
+      </c>
+      <c r="N6" t="str">
+        <v>591.64</v>
+      </c>
+      <c r="O6" t="str">
+        <v>0.10</v>
+      </c>
+      <c r="P6" t="str">
+        <v>870.30</v>
+      </c>
+      <c r="Q6" t="str">
+        <v>1576.00</v>
+      </c>
+      <c r="R6" t="str">
+        <v>No</v>
+      </c>
+      <c r="S6" t="str">
+        <v>711.94</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="str">
+        <v>Scenario 1 - Gradual Increase</v>
+      </c>
+      <c r="B7">
+        <v>6</v>
+      </c>
+      <c r="C7">
+        <v>2800</v>
+      </c>
+      <c r="D7" t="str">
+        <v>150.00</v>
+      </c>
+      <c r="E7" t="str">
+        <v>0.365260</v>
+      </c>
+      <c r="F7" t="str">
+        <v>0.367506</v>
+      </c>
+      <c r="G7" t="str">
+        <v>1029.02</v>
+      </c>
+      <c r="H7" t="str">
+        <v>132.69</v>
+      </c>
+      <c r="I7" t="str">
+        <v>732.45</v>
+      </c>
+      <c r="J7" t="str">
+        <v>8.17</v>
+      </c>
+      <c r="K7" t="str">
+        <v>45.08</v>
+      </c>
+      <c r="L7" t="str">
+        <v>728.63</v>
+      </c>
+      <c r="M7" t="str">
+        <v>0.72</v>
+      </c>
+      <c r="N7" t="str">
+        <v>723.37</v>
+      </c>
+      <c r="O7" t="str">
+        <v>0.10</v>
+      </c>
+      <c r="P7" t="str">
+        <v>1019.83</v>
+      </c>
+      <c r="Q7" t="str">
+        <v>1644.25</v>
+      </c>
+      <c r="R7" t="str">
+        <v>No</v>
+      </c>
+      <c r="S7" t="str">
+        <v>843.20</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="str">
+        <v>Scenario 1 - Gradual Increase</v>
+      </c>
+      <c r="B8">
+        <v>7</v>
+      </c>
+      <c r="C8">
+        <v>3300</v>
+      </c>
+      <c r="D8" t="str">
+        <v>150.00</v>
+      </c>
+      <c r="E8" t="str">
+        <v>0.410714</v>
+      </c>
+      <c r="F8" t="str">
+        <v>0.413649</v>
+      </c>
+      <c r="G8" t="str">
+        <v>1365.04</v>
+      </c>
+      <c r="H8" t="str">
+        <v>209.70</v>
+      </c>
+      <c r="I8" t="str">
+        <v>943.72</v>
+      </c>
+      <c r="J8" t="str">
+        <v>10.02</v>
+      </c>
+      <c r="K8" t="str">
+        <v>45.08</v>
+      </c>
+      <c r="L8" t="str">
+        <v>938.33</v>
+      </c>
+      <c r="M8" t="str">
+        <v>2.02</v>
+      </c>
+      <c r="N8" t="str">
+        <v>919.38</v>
+      </c>
+      <c r="O8" t="str">
+        <v>0.10</v>
+      </c>
+      <c r="P8" t="str">
+        <v>1340.60</v>
+      </c>
+      <c r="Q8" t="str">
+        <v>1882.20</v>
+      </c>
+      <c r="R8" t="str">
+        <v>No</v>
+      </c>
+      <c r="S8" t="str">
+        <v>1209.97</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="str">
+        <v>Scenario 1 - Gradual Increase</v>
+      </c>
+      <c r="B9">
+        <v>8</v>
+      </c>
+      <c r="C9">
+        <v>3300</v>
+      </c>
+      <c r="D9" t="str">
+        <v>150.00</v>
+      </c>
+      <c r="E9" t="str">
+        <v>0.456169</v>
+      </c>
+      <c r="F9" t="str">
+        <v>0.459869</v>
+      </c>
+      <c r="G9" t="str">
+        <v>1517.57</v>
+      </c>
+      <c r="H9" t="str">
+        <v>161.43</v>
+      </c>
+      <c r="I9" t="str">
+        <v>1107.00</v>
+      </c>
+      <c r="J9" t="str">
+        <v>6.57</v>
+      </c>
+      <c r="K9" t="str">
+        <v>45.07</v>
+      </c>
+      <c r="L9" t="str">
+        <v>1099.77</v>
+      </c>
+      <c r="M9" t="str">
+        <v>2.02</v>
+      </c>
+      <c r="N9" t="str">
+        <v>1077.55</v>
+      </c>
+      <c r="O9" t="str">
+        <v>0.10</v>
+      </c>
+      <c r="P9" t="str">
+        <v>1488.02</v>
+      </c>
+      <c r="Q9" t="str">
+        <v>1985.94</v>
+      </c>
+      <c r="R9" t="str">
+        <v>No</v>
+      </c>
+      <c r="S9" t="str">
+        <v>1365.56</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="str">
+        <v>Scenario 1 - Gradual Increase</v>
+      </c>
+      <c r="B10">
+        <v>9</v>
+      </c>
+      <c r="C10">
+        <v>3300</v>
+      </c>
+      <c r="D10" t="str">
+        <v>150.00</v>
+      </c>
+      <c r="E10" t="str">
+        <v>0.501623</v>
+      </c>
+      <c r="F10" t="str">
+        <v>0.506166</v>
+      </c>
+      <c r="G10" t="str">
+        <v>1670.35</v>
+      </c>
+      <c r="H10" t="str">
+        <v>139.55</v>
+      </c>
+      <c r="I10" t="str">
+        <v>1248.63</v>
+      </c>
+      <c r="J10" t="str">
+        <v>5.04</v>
+      </c>
+      <c r="K10" t="str">
+        <v>45.08</v>
+      </c>
+      <c r="L10" t="str">
+        <v>1239.32</v>
+      </c>
+      <c r="M10" t="str">
+        <v>2.02</v>
+      </c>
+      <c r="N10" t="str">
+        <v>1214.28</v>
+      </c>
+      <c r="O10" t="str">
+        <v>0.10</v>
+      </c>
+      <c r="P10" t="str">
+        <v>1635.90</v>
+      </c>
+      <c r="Q10" t="str">
+        <v>2035.14</v>
+      </c>
+      <c r="R10" t="str">
+        <v>No</v>
+      </c>
+      <c r="S10" t="str">
+        <v>1500.18</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="str">
+        <v>Scenario 1 - Gradual Increase</v>
+      </c>
+      <c r="B11">
+        <v>10</v>
+      </c>
+      <c r="C11">
+        <v>4000</v>
+      </c>
+      <c r="D11" t="str">
+        <v>150.00</v>
+      </c>
+      <c r="E11" t="str">
+        <v>0.539123</v>
+      </c>
+      <c r="F11" t="str">
+        <v>0.544572</v>
+      </c>
+      <c r="G11" t="str">
+        <v>2178.29</v>
+      </c>
+      <c r="H11" t="str">
+        <v>289.29</v>
+      </c>
+      <c r="I11" t="str">
+        <v>1540.49</v>
+      </c>
+      <c r="J11" t="str">
+        <v>8.46</v>
+      </c>
+      <c r="K11" t="str">
+        <v>45.08</v>
+      </c>
+      <c r="L11" t="str">
+        <v>1528.61</v>
+      </c>
+      <c r="M11" t="str">
+        <v>4.31</v>
+      </c>
+      <c r="N11" t="str">
+        <v>1462.78</v>
+      </c>
+      <c r="O11" t="str">
+        <v>0.10</v>
+      </c>
+      <c r="P11" t="str">
+        <v>2100.48</v>
+      </c>
+      <c r="Q11" t="str">
+        <v>2333.76</v>
+      </c>
+      <c r="R11" t="str">
+        <v>No</v>
+      </c>
+      <c r="S11" t="str">
+        <v>2063.25</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="str">
+        <v>Scenario 1 - Gradual Increase</v>
+      </c>
+      <c r="B12">
+        <v>11</v>
+      </c>
+      <c r="C12">
+        <v>4000</v>
+      </c>
+      <c r="D12" t="str">
+        <v>150.00</v>
+      </c>
+      <c r="E12" t="str">
+        <v>0.576623</v>
+      </c>
+      <c r="F12" t="str">
+        <v>0.583042</v>
+      </c>
+      <c r="G12" t="str">
+        <v>2332.17</v>
+      </c>
+      <c r="H12" t="str">
+        <v>196.87</v>
+      </c>
+      <c r="I12" t="str">
+        <v>1740.25</v>
+      </c>
+      <c r="J12" t="str">
+        <v>5.10</v>
+      </c>
+      <c r="K12" t="str">
+        <v>45.07</v>
+      </c>
+      <c r="L12" t="str">
+        <v>1725.48</v>
+      </c>
+      <c r="M12" t="str">
+        <v>4.31</v>
+      </c>
+      <c r="N12" t="str">
+        <v>1651.16</v>
+      </c>
+      <c r="O12" t="str">
+        <v>0.10</v>
+      </c>
+      <c r="P12" t="str">
+        <v>2242.98</v>
+      </c>
+      <c r="Q12" t="str">
+        <v>2462.44</v>
+      </c>
+      <c r="R12" t="str">
+        <v>No</v>
+      </c>
+      <c r="S12" t="str">
+        <v>2244.14</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="str">
+        <v>Scenario 1 - Gradual Increase</v>
+      </c>
+      <c r="B13">
+        <v>12</v>
+      </c>
+      <c r="C13">
+        <v>4000</v>
+      </c>
+      <c r="D13" t="str">
+        <v>150.00</v>
+      </c>
+      <c r="E13" t="str">
+        <v>0.614123</v>
+      </c>
+      <c r="F13" t="str">
+        <v>0.621576</v>
+      </c>
+      <c r="G13" t="str">
+        <v>2486.30</v>
+      </c>
+      <c r="H13" t="str">
+        <v>155.06</v>
+      </c>
+      <c r="I13" t="str">
+        <v>1898.46</v>
+      </c>
+      <c r="J13" t="str">
+        <v>3.68</v>
+      </c>
+      <c r="K13" t="str">
+        <v>45.08</v>
+      </c>
+      <c r="L13" t="str">
+        <v>1880.54</v>
+      </c>
+      <c r="M13" t="str">
+        <v>4.31</v>
+      </c>
+      <c r="N13" t="str">
+        <v>1799.54</v>
+      </c>
+      <c r="O13" t="str">
+        <v>0.10</v>
+      </c>
+      <c r="P13" t="str">
+        <v>2387.28</v>
+      </c>
+      <c r="Q13" t="str">
+        <v>2519.77</v>
+      </c>
+      <c r="R13" t="str">
+        <v>No</v>
+      </c>
+      <c r="S13" t="str">
+        <v>2386.82</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="str">
+        <v>Scenario 2 - Gradual Decrease</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14">
+        <v>4000</v>
+      </c>
+      <c r="D14" t="str">
+        <v>150.00</v>
+      </c>
+      <c r="E14" t="str">
+        <v>0.037500</v>
+      </c>
+      <c r="F14" t="str">
+        <v>0.037562</v>
+      </c>
+      <c r="G14" t="str">
+        <v>150.25</v>
+      </c>
+      <c r="H14" t="str">
+        <v>67.61</v>
+      </c>
+      <c r="I14" t="str">
+        <v>67.73</v>
+      </c>
+      <c r="J14" t="str">
+        <v>45.00</v>
+      </c>
+      <c r="K14" t="str">
+        <v>45.08</v>
+      </c>
+      <c r="L14" t="str">
+        <v>67.61</v>
+      </c>
+      <c r="M14" t="str">
+        <v>4.31</v>
+      </c>
+      <c r="N14" t="str">
+        <v>64.70</v>
+      </c>
+      <c r="O14" t="str">
+        <v>0.10</v>
+      </c>
+      <c r="P14" t="str">
+        <v>147.13</v>
+      </c>
+      <c r="Q14" t="str">
+        <v>1487.48</v>
+      </c>
+      <c r="R14" t="str">
+        <v>No</v>
+      </c>
+      <c r="S14" t="str">
+        <v>61.83</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="str">
+        <v>Scenario 2 - Gradual Decrease</v>
+      </c>
+      <c r="B15">
+        <v>2</v>
+      </c>
+      <c r="C15">
+        <v>4000</v>
+      </c>
+      <c r="D15" t="str">
+        <v>150.00</v>
+      </c>
+      <c r="E15" t="str">
+        <v>0.075000</v>
+      </c>
+      <c r="F15" t="str">
+        <v>0.075188</v>
+      </c>
+      <c r="G15" t="str">
+        <v>300.75</v>
+      </c>
+      <c r="H15" t="str">
+        <v>98.04</v>
+      </c>
+      <c r="I15" t="str">
+        <v>166.04</v>
+      </c>
+      <c r="J15" t="str">
+        <v>26.61</v>
+      </c>
+      <c r="K15" t="str">
+        <v>45.08</v>
+      </c>
+      <c r="L15" t="str">
+        <v>165.65</v>
+      </c>
+      <c r="M15" t="str">
+        <v>4.31</v>
+      </c>
+      <c r="N15" t="str">
+        <v>158.52</v>
+      </c>
+      <c r="O15" t="str">
+        <v>0.10</v>
+      </c>
+      <c r="P15" t="str">
+        <v>293.13</v>
+      </c>
+      <c r="Q15" t="str">
+        <v>1821.88</v>
+      </c>
+      <c r="R15" t="str">
+        <v>No</v>
+      </c>
+      <c r="S15" t="str">
+        <v>151.64</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="str">
+        <v>Scenario 2 - Gradual Decrease</v>
+      </c>
+      <c r="B16">
+        <v>3</v>
+      </c>
+      <c r="C16">
+        <v>4000</v>
+      </c>
+      <c r="D16" t="str">
+        <v>150.00</v>
+      </c>
+      <c r="E16" t="str">
+        <v>0.112500</v>
+      </c>
+      <c r="F16" t="str">
+        <v>0.112875</v>
+      </c>
+      <c r="G16" t="str">
+        <v>451.50</v>
+      </c>
+      <c r="H16" t="str">
+        <v>111.68</v>
+      </c>
+      <c r="I16" t="str">
+        <v>278.18</v>
+      </c>
+      <c r="J16" t="str">
+        <v>18.10</v>
+      </c>
+      <c r="K16" t="str">
+        <v>45.08</v>
+      </c>
+      <c r="L16" t="str">
+        <v>277.33</v>
+      </c>
+      <c r="M16" t="str">
+        <v>4.31</v>
+      </c>
+      <c r="N16" t="str">
+        <v>265.38</v>
+      </c>
+      <c r="O16" t="str">
+        <v>0.10</v>
+      </c>
+      <c r="P16" t="str">
+        <v>438.60</v>
+      </c>
+      <c r="Q16" t="str">
+        <v>2033.21</v>
+      </c>
+      <c r="R16" t="str">
+        <v>No</v>
+      </c>
+      <c r="S16" t="str">
+        <v>253.99</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="str">
+        <v>Scenario 2 - Gradual Decrease</v>
+      </c>
+      <c r="B17">
+        <v>4</v>
+      </c>
+      <c r="C17">
+        <v>3300</v>
+      </c>
+      <c r="D17" t="str">
+        <v>150.00</v>
+      </c>
+      <c r="E17" t="str">
+        <v>0.157955</v>
+      </c>
+      <c r="F17" t="str">
+        <v>0.158594</v>
+      </c>
+      <c r="G17" t="str">
+        <v>523.36</v>
+      </c>
+      <c r="H17" t="str">
+        <v>82.13</v>
+      </c>
+      <c r="I17" t="str">
+        <v>360.91</v>
+      </c>
+      <c r="J17" t="str">
+        <v>10.26</v>
+      </c>
+      <c r="K17" t="str">
+        <v>45.08</v>
+      </c>
+      <c r="L17" t="str">
+        <v>359.46</v>
+      </c>
+      <c r="M17" t="str">
+        <v>2.02</v>
+      </c>
+      <c r="N17" t="str">
+        <v>352.20</v>
+      </c>
+      <c r="O17" t="str">
+        <v>0.10</v>
+      </c>
+      <c r="P17" t="str">
+        <v>514.54</v>
+      </c>
+      <c r="Q17" t="str">
+        <v>1877.45</v>
+      </c>
+      <c r="R17" t="str">
+        <v>No</v>
+      </c>
+      <c r="S17" t="str">
+        <v>266.74</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="str">
+        <v>Scenario 2 - Gradual Decrease</v>
+      </c>
+      <c r="B18">
+        <v>5</v>
+      </c>
+      <c r="C18">
+        <v>3300</v>
+      </c>
+      <c r="D18" t="str">
+        <v>150.00</v>
+      </c>
+      <c r="E18" t="str">
+        <v>0.203409</v>
+      </c>
+      <c r="F18" t="str">
+        <v>0.204388</v>
+      </c>
+      <c r="G18" t="str">
+        <v>674.48</v>
+      </c>
+      <c r="H18" t="str">
+        <v>104.36</v>
+      </c>
+      <c r="I18" t="str">
+        <v>466.05</v>
+      </c>
+      <c r="J18" t="str">
+        <v>10.09</v>
+      </c>
+      <c r="K18" t="str">
+        <v>45.08</v>
+      </c>
+      <c r="L18" t="str">
+        <v>463.82</v>
+      </c>
+      <c r="M18" t="str">
+        <v>2.02</v>
+      </c>
+      <c r="N18" t="str">
+        <v>454.45</v>
+      </c>
+      <c r="O18" t="str">
+        <v>0.10</v>
+      </c>
+      <c r="P18" t="str">
+        <v>662.78</v>
+      </c>
+      <c r="Q18" t="str">
+        <v>1881.17</v>
+      </c>
+      <c r="R18" t="str">
+        <v>No</v>
+      </c>
+      <c r="S18" t="str">
+        <v>367.23</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="str">
+        <v>Scenario 2 - Gradual Decrease</v>
+      </c>
+      <c r="B19">
+        <v>6</v>
+      </c>
+      <c r="C19">
+        <v>3300</v>
+      </c>
+      <c r="D19" t="str">
+        <v>150.00</v>
+      </c>
+      <c r="E19" t="str">
+        <v>0.248864</v>
+      </c>
+      <c r="F19" t="str">
+        <v>0.250259</v>
+      </c>
+      <c r="G19" t="str">
+        <v>825.86</v>
+      </c>
+      <c r="H19" t="str">
+        <v>114.31</v>
+      </c>
+      <c r="I19" t="str">
+        <v>581.32</v>
+      </c>
+      <c r="J19" t="str">
+        <v>8.86</v>
+      </c>
+      <c r="K19" t="str">
+        <v>45.08</v>
+      </c>
+      <c r="L19" t="str">
+        <v>578.13</v>
+      </c>
+      <c r="M19" t="str">
+        <v>2.02</v>
+      </c>
+      <c r="N19" t="str">
+        <v>566.45</v>
+      </c>
+      <c r="O19" t="str">
+        <v>0.10</v>
+      </c>
+      <c r="P19" t="str">
+        <v>810.88</v>
+      </c>
+      <c r="Q19" t="str">
+        <v>1916.37</v>
+      </c>
+      <c r="R19" t="str">
+        <v>No</v>
+      </c>
+      <c r="S19" t="str">
+        <v>477.33</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="str">
+        <v>Scenario 2 - Gradual Decrease</v>
+      </c>
+      <c r="B20">
+        <v>7</v>
+      </c>
+      <c r="C20">
+        <v>2800</v>
+      </c>
+      <c r="D20" t="str">
+        <v>150.00</v>
+      </c>
+      <c r="E20" t="str">
+        <v>0.302435</v>
+      </c>
+      <c r="F20" t="str">
+        <v>0.304337</v>
+      </c>
+      <c r="G20" t="str">
+        <v>852.14</v>
+      </c>
+      <c r="H20" t="str">
+        <v>62.30</v>
+      </c>
+      <c r="I20" t="str">
+        <v>644.69</v>
+      </c>
+      <c r="J20" t="str">
+        <v>4.36</v>
+      </c>
+      <c r="K20" t="str">
+        <v>45.08</v>
+      </c>
+      <c r="L20" t="str">
+        <v>640.43</v>
+      </c>
+      <c r="M20" t="str">
+        <v>0.72</v>
+      </c>
+      <c r="N20" t="str">
+        <v>635.80</v>
+      </c>
+      <c r="O20" t="str">
+        <v>0.10</v>
+      </c>
+      <c r="P20" t="str">
+        <v>843.15</v>
+      </c>
+      <c r="Q20" t="str">
+        <v>1747.64</v>
+      </c>
+      <c r="R20" t="str">
+        <v>No</v>
+      </c>
+      <c r="S20" t="str">
+        <v>428.95</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="str">
+        <v>Scenario 2 - Gradual Decrease</v>
+      </c>
+      <c r="B21">
+        <v>8</v>
+      </c>
+      <c r="C21">
+        <v>2800</v>
+      </c>
+      <c r="D21" t="str">
+        <v>150.00</v>
+      </c>
+      <c r="E21" t="str">
+        <v>0.356006</v>
+      </c>
+      <c r="F21" t="str">
+        <v>0.358505</v>
+      </c>
+      <c r="G21" t="str">
+        <v>1003.81</v>
+      </c>
+      <c r="H21" t="str">
+        <v>95.21</v>
+      </c>
+      <c r="I21" t="str">
+        <v>741.14</v>
+      </c>
+      <c r="J21" t="str">
+        <v>5.79</v>
+      </c>
+      <c r="K21" t="str">
+        <v>45.07</v>
+      </c>
+      <c r="L21" t="str">
+        <v>735.64</v>
+      </c>
+      <c r="M21" t="str">
+        <v>0.72</v>
+      </c>
+      <c r="N21" t="str">
+        <v>730.33</v>
+      </c>
+      <c r="O21" t="str">
+        <v>0.10</v>
+      </c>
+      <c r="P21" t="str">
+        <v>992.90</v>
+      </c>
+      <c r="Q21" t="str">
+        <v>1705.53</v>
+      </c>
+      <c r="R21" t="str">
+        <v>No</v>
+      </c>
+      <c r="S21" t="str">
+        <v>523.22</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="str">
+        <v>Scenario 2 - Gradual Decrease</v>
+      </c>
+      <c r="B22">
+        <v>9</v>
+      </c>
+      <c r="C22">
+        <v>2800</v>
+      </c>
+      <c r="D22" t="str">
+        <v>150.00</v>
+      </c>
+      <c r="E22" t="str">
+        <v>0.409578</v>
+      </c>
+      <c r="F22" t="str">
+        <v>0.412763</v>
+      </c>
+      <c r="G22" t="str">
+        <v>1155.74</v>
+      </c>
+      <c r="H22" t="str">
+        <v>109.98</v>
+      </c>
+      <c r="I22" t="str">
+        <v>852.54</v>
+      </c>
+      <c r="J22" t="str">
+        <v>5.81</v>
+      </c>
+      <c r="K22" t="str">
+        <v>45.08</v>
+      </c>
+      <c r="L22" t="str">
+        <v>845.62</v>
+      </c>
+      <c r="M22" t="str">
+        <v>0.72</v>
+      </c>
+      <c r="N22" t="str">
+        <v>839.51</v>
+      </c>
+      <c r="O22" t="str">
+        <v>0.10</v>
+      </c>
+      <c r="P22" t="str">
+        <v>1142.61</v>
+      </c>
+      <c r="Q22" t="str">
+        <v>1703.99</v>
+      </c>
+      <c r="R22" t="str">
+        <v>No</v>
+      </c>
+      <c r="S22" t="str">
+        <v>632.12</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="str">
+        <v>Scenario 2 - Gradual Decrease</v>
+      </c>
+      <c r="B23">
+        <v>10</v>
+      </c>
+      <c r="C23">
+        <v>2200</v>
+      </c>
+      <c r="D23" t="str">
+        <v>150.00</v>
+      </c>
+      <c r="E23" t="str">
+        <v>0.477760</v>
+      </c>
+      <c r="F23" t="str">
+        <v>0.481747</v>
+      </c>
+      <c r="G23" t="str">
+        <v>1059.84</v>
+      </c>
+      <c r="H23" t="str">
+        <v>4.92</v>
+      </c>
+      <c r="I23" t="str">
+        <v>858.89</v>
+      </c>
+      <c r="J23" t="str">
+        <v>0.26</v>
+      </c>
+      <c r="K23" t="str">
+        <v>45.08</v>
+      </c>
+      <c r="L23" t="str">
+        <v>850.54</v>
+      </c>
+      <c r="M23" t="str">
+        <v>0.00</v>
+      </c>
+      <c r="N23" t="str">
+        <v>850.54</v>
+      </c>
+      <c r="O23" t="str">
+        <v>0.10</v>
+      </c>
+      <c r="P23" t="str">
+        <v>1051.39</v>
+      </c>
+      <c r="Q23" t="str">
+        <v>1470.86</v>
+      </c>
+      <c r="R23" t="str">
+        <v>No</v>
+      </c>
+      <c r="S23" t="str">
+        <v>401.93</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="str">
+        <v>Scenario 2 - Gradual Decrease</v>
+      </c>
+      <c r="B24">
+        <v>11</v>
+      </c>
+      <c r="C24">
+        <v>2200</v>
+      </c>
+      <c r="D24" t="str">
+        <v>150.00</v>
+      </c>
+      <c r="E24" t="str">
+        <v>0.545942</v>
+      </c>
+      <c r="F24" t="str">
+        <v>0.550845</v>
+      </c>
+      <c r="G24" t="str">
+        <v>1211.86</v>
+      </c>
+      <c r="H24" t="str">
+        <v>69.19</v>
+      </c>
+      <c r="I24" t="str">
+        <v>929.63</v>
+      </c>
+      <c r="J24" t="str">
+        <v>3.35</v>
+      </c>
+      <c r="K24" t="str">
+        <v>45.07</v>
+      </c>
+      <c r="L24" t="str">
+        <v>919.73</v>
+      </c>
+      <c r="M24" t="str">
+        <v>0.00</v>
+      </c>
+      <c r="N24" t="str">
+        <v>919.73</v>
+      </c>
+      <c r="O24" t="str">
+        <v>0.10</v>
+      </c>
+      <c r="P24" t="str">
+        <v>1201.86</v>
+      </c>
+      <c r="Q24" t="str">
+        <v>1392.30</v>
+      </c>
+      <c r="R24" t="str">
+        <v>No</v>
+      </c>
+      <c r="S24" t="str">
+        <v>471.59</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="str">
+        <v>Scenario 2 - Gradual Decrease</v>
+      </c>
+      <c r="B25">
+        <v>12</v>
+      </c>
+      <c r="C25">
+        <v>2200</v>
+      </c>
+      <c r="D25" t="str">
+        <v>150.00</v>
+      </c>
+      <c r="E25" t="str">
+        <v>0.614123</v>
+      </c>
+      <c r="F25" t="str">
+        <v>0.620059</v>
+      </c>
+      <c r="G25" t="str">
+        <v>1364.13</v>
+      </c>
+      <c r="H25" t="str">
+        <v>98.11</v>
+      </c>
+      <c r="I25" t="str">
+        <v>1029.45</v>
+      </c>
+      <c r="J25" t="str">
+        <v>4.30</v>
+      </c>
+      <c r="K25" t="str">
+        <v>45.08</v>
+      </c>
+      <c r="L25" t="str">
+        <v>1017.84</v>
+      </c>
+      <c r="M25" t="str">
+        <v>0.00</v>
+      </c>
+      <c r="N25" t="str">
+        <v>1017.84</v>
+      </c>
+      <c r="O25" t="str">
+        <v>0.10</v>
+      </c>
+      <c r="P25" t="str">
+        <v>1352.42</v>
+      </c>
+      <c r="Q25" t="str">
+        <v>1369.70</v>
+      </c>
+      <c r="R25" t="str">
+        <v>No</v>
+      </c>
+      <c r="S25" t="str">
+        <v>570.26</v>
+      </c>
+    </row>
+  </sheetData>
+  <ignoredErrors>
+    <ignoredError numberStoredAsText="1" sqref="A1:S25"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>